<commit_message>
major changes upto combining table
</commit_message>
<xml_diff>
--- a/csv files/stations/missing_stations.xlsx
+++ b/csv files/stations/missing_stations.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\divvy-bikeshare\csv files\stations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2B0993E3-0CF7-4D53-A1DA-88879DBB9CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EA55D5-7168-438B-AD90-6B19A19D916A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11760" yWindow="180" windowWidth="11535" windowHeight="14445"/>
+    <workbookView xWindow="-28710" yWindow="480" windowWidth="10950" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="missing_stations" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,23 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">missing_stations!$A$1:$G$58</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Query - Divvy_Bicycle_Stations" description="Connection to the 'Divvy_Bicycle_Stations' query in the workbook." type="5" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Query - Divvy_Bicycle_Stations" description="Connection to the 'Divvy_Bicycle_Stations' query in the workbook." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Divvy_Bicycle_Stations;Extended Properties=&quot;&quot;" command="SELECT * FROM [Divvy_Bicycle_Stations]"/>
   </connection>
 </connections>
@@ -7783,7 +7793,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -8794,12 +8804,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8836,26 +8846,26 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>651</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="C2" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A2,Stations!A:A,1,FALSE)=A2,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B2,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>674</v>
+        <v>not found</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>459</v>
+        <v>357</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="C3" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A3,Stations!A:A,1,FALSE)=A3,"taken"),"free")</f>
@@ -8863,15 +8873,15 @@
       </c>
       <c r="D3">
         <f>_xlfn.IFNA(VLOOKUP(B3,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>760</v>
+        <v>1.56E+18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A4,Stations!A:A,1,FALSE)=A4,"taken"),"free")</f>
@@ -8884,10 +8894,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A5,Stations!A:A,1,FALSE)=A5,"taken"),"free")</f>
@@ -8897,13 +8907,16 @@
         <f>_xlfn.IFNA(VLOOKUP(B5,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
         <v>1.56E+18</v>
       </c>
+      <c r="G5" t="s">
+        <v>2579</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A6,Stations!A:A,1,FALSE)=A6,"taken"),"free")</f>
@@ -8919,10 +8932,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A7,Stations!A:A,1,FALSE)=A7,"taken"),"free")</f>
@@ -8932,16 +8945,13 @@
         <f>_xlfn.IFNA(VLOOKUP(B7,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
         <v>1.56E+18</v>
       </c>
-      <c r="G7" t="s">
-        <v>2579</v>
-      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A8,Stations!A:A,1,FALSE)=A8,"taken"),"free")</f>
@@ -8951,13 +8961,16 @@
         <f>_xlfn.IFNA(VLOOKUP(B8,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
         <v>1.56E+18</v>
       </c>
+      <c r="G8" t="s">
+        <v>2579</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>363</v>
+        <v>371</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C9" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A9,Stations!A:A,1,FALSE)=A9,"taken"),"free")</f>
@@ -8965,53 +8978,53 @@
       </c>
       <c r="D9">
         <f>_xlfn.IFNA(VLOOKUP(B9,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.56E+18</v>
-      </c>
-      <c r="G9" t="s">
-        <v>2579</v>
+        <v>1.58E+18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>473</v>
+        <v>372</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="C10" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A10,Stations!A:A,1,FALSE)=A10,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B10,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.56E+18</v>
+        <v>not found</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1195</v>
+      </c>
+      <c r="F10">
+        <v>622</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>397</v>
+        <v>372</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="C11" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A11,Stations!A:A,1,FALSE)=A11,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B11,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.57E+18</v>
-      </c>
-      <c r="G11" t="s">
-        <v>2579</v>
+        <v>not found</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>371</v>
+        <v>379</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A12,Stations!A:A,1,FALSE)=A12,"taken"),"free")</f>
@@ -9024,10 +9037,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A13,Stations!A:A,1,FALSE)=A13,"taken"),"free")</f>
@@ -9040,10 +9053,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C14" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A14,Stations!A:A,1,FALSE)=A14,"taken"),"free")</f>
@@ -9056,10 +9069,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A15,Stations!A:A,1,FALSE)=A15,"taken"),"free")</f>
@@ -9072,10 +9085,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>389</v>
+        <v>397</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A16,Stations!A:A,1,FALSE)=A16,"taken"),"free")</f>
@@ -9083,85 +9096,85 @@
       </c>
       <c r="D16">
         <f>_xlfn.IFNA(VLOOKUP(B16,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.58E+18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.57E+18</v>
+      </c>
+      <c r="G16" t="s">
+        <v>2579</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="C17" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A17,Stations!A:A,1,FALSE)=A17,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D17">
+      <c r="D17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B17,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.59E+18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>not found</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2581</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1</v>
+        <v>404</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="C18" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A18,Stations!A:A,1,FALSE)=A18,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D18" t="str">
+      <c r="D18">
         <f>_xlfn.IFNA(VLOOKUP(B18,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>not found</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.59E+18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>372</v>
+        <v>459</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C19" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A19,Stations!A:A,1,FALSE)=A19,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D19" t="str">
+      <c r="D19">
         <f>_xlfn.IFNA(VLOOKUP(B19,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>not found</v>
-      </c>
-      <c r="E19" t="s">
-        <v>1195</v>
-      </c>
-      <c r="F19">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>372</v>
+        <v>473</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="C20" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A20,Stations!A:A,1,FALSE)=A20,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D20" t="str">
+      <c r="D20">
         <f>_xlfn.IFNA(VLOOKUP(B20,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>not found</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.56E+18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>397</v>
+        <v>512</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C21" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A21,Stations!A:A,1,FALSE)=A21,"taken"),"free")</f>
@@ -9171,16 +9184,13 @@
         <f>_xlfn.IFNA(VLOOKUP(B21,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
         <v>not found</v>
       </c>
-      <c r="E21" t="s">
-        <v>2581</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>512</v>
+        <v>606</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C22" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A22,Stations!A:A,1,FALSE)=A22,"taken"),"free")</f>
@@ -9191,12 +9201,12 @@
         <v>not found</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C23" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A23,Stations!A:A,1,FALSE)=A23,"taken"),"free")</f>
@@ -9207,12 +9217,12 @@
         <v>not found</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C24" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A24,Stations!A:A,1,FALSE)=A24,"taken"),"free")</f>
@@ -9223,12 +9233,12 @@
         <v>not found</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C25" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A25,Stations!A:A,1,FALSE)=A25,"taken"),"free")</f>
@@ -9239,12 +9249,12 @@
         <v>not found</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C26" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A26,Stations!A:A,1,FALSE)=A26,"taken"),"free")</f>
@@ -9255,12 +9265,12 @@
         <v>not found</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C27" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A27,Stations!A:A,1,FALSE)=A27,"taken"),"free")</f>
@@ -9271,12 +9281,12 @@
         <v>not found</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C28" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A28,Stations!A:A,1,FALSE)=A28,"taken"),"free")</f>
@@ -9287,12 +9297,12 @@
         <v>not found</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C29" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A29,Stations!A:A,1,FALSE)=A29,"taken"),"free")</f>
@@ -9303,12 +9313,12 @@
         <v>not found</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>613</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C30" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A30,Stations!A:A,1,FALSE)=A30,"taken"),"free")</f>
@@ -9318,13 +9328,16 @@
         <f>_xlfn.IFNA(VLOOKUP(B30,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
         <v>not found</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C31" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A31,Stations!A:A,1,FALSE)=A31,"taken"),"free")</f>
@@ -9334,16 +9347,13 @@
         <f>_xlfn.IFNA(VLOOKUP(B31,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
         <v>not found</v>
       </c>
-      <c r="E31" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C32" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A32,Stations!A:A,1,FALSE)=A32,"taken"),"free")</f>
@@ -9356,10 +9366,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C33" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A33,Stations!A:A,1,FALSE)=A33,"taken"),"free")</f>
@@ -9372,10 +9382,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B34" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C34" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A34,Stations!A:A,1,FALSE)=A34,"taken"),"free")</f>
@@ -9388,10 +9398,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C35" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A35,Stations!A:A,1,FALSE)=A35,"taken"),"free")</f>
@@ -9404,18 +9414,18 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>618</v>
+        <v>651</v>
       </c>
       <c r="B36" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C36" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A36,Stations!A:A,1,FALSE)=A36,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D36" t="str">
+      <c r="D36">
         <f>_xlfn.IFNA(VLOOKUP(B36,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>not found</v>
+        <v>674</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -9503,7 +9513,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C42" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A42,Stations!A:A,1,FALSE)=A42,"taken"),"free")</f>
@@ -9516,7 +9526,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C43" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A43,Stations!A:A,1,FALSE)=A43,"taken"),"free")</f>
@@ -9765,7 +9775,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G58">
+  <autoFilter ref="A1:G58" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G58">
       <sortCondition ref="C1:C58"/>
     </sortState>
@@ -9807,7 +9817,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G1270"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
working at combine stations
</commit_message>
<xml_diff>
--- a/csv files/stations/missing_stations.xlsx
+++ b/csv files/stations/missing_stations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\divvy-bikeshare\csv files\stations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EA55D5-7168-438B-AD90-6B19A19D916A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B403AE27-2F74-4948-B80E-841FC722682B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28710" yWindow="480" windowWidth="10950" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="315" yWindow="1005" windowWidth="12480" windowHeight="14445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="missing_stations" sheetId="1" r:id="rId1"/>
@@ -8808,7 +8808,7 @@
   <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -8846,26 +8846,26 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>651</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C2" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A2,Stations!A:A,1,FALSE)=A2,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D2" t="str">
+      <c r="D2">
         <f>_xlfn.IFNA(VLOOKUP(B2,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>not found</v>
+        <v>674</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>357</v>
+        <v>459</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C3" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A3,Stations!A:A,1,FALSE)=A3,"taken"),"free")</f>
@@ -8873,31 +8873,31 @@
       </c>
       <c r="D3">
         <f>_xlfn.IFNA(VLOOKUP(B3,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.56E+18</v>
+        <v>760</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>358</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C4" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A4,Stations!A:A,1,FALSE)=A4,"taken"),"free")</f>
-        <v>free</v>
+        <v>taken</v>
       </c>
       <c r="D4">
         <f>_xlfn.IFNA(VLOOKUP(B4,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.56E+18</v>
+        <v>1.52E+18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A5,Stations!A:A,1,FALSE)=A5,"taken"),"free")</f>
@@ -8907,16 +8907,13 @@
         <f>_xlfn.IFNA(VLOOKUP(B5,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
         <v>1.56E+18</v>
       </c>
-      <c r="G5" t="s">
-        <v>2579</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A6,Stations!A:A,1,FALSE)=A6,"taken"),"free")</f>
@@ -8926,16 +8923,13 @@
         <f>_xlfn.IFNA(VLOOKUP(B6,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
         <v>1.56E+18</v>
       </c>
-      <c r="G6" t="s">
-        <v>2579</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A7,Stations!A:A,1,FALSE)=A7,"taken"),"free")</f>
@@ -8945,13 +8939,16 @@
         <f>_xlfn.IFNA(VLOOKUP(B7,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
         <v>1.56E+18</v>
       </c>
+      <c r="G7" t="s">
+        <v>2579</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C8" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A8,Stations!A:A,1,FALSE)=A8,"taken"),"free")</f>
@@ -8967,10 +8964,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A9,Stations!A:A,1,FALSE)=A9,"taken"),"free")</f>
@@ -8978,331 +8975,325 @@
       </c>
       <c r="D9">
         <f>_xlfn.IFNA(VLOOKUP(B9,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.58E+18</v>
+        <v>1.56E+18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C10" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A10,Stations!A:A,1,FALSE)=A10,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D10" t="str">
+      <c r="D10">
         <f>_xlfn.IFNA(VLOOKUP(B10,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>not found</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1195</v>
-      </c>
-      <c r="F10">
-        <v>622</v>
+        <v>1.56E+18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>2579</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>372</v>
+        <v>473</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="C11" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A11,Stations!A:A,1,FALSE)=A11,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D11" t="str">
+      <c r="D11">
         <f>_xlfn.IFNA(VLOOKUP(B11,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>not found</v>
+        <v>1.56E+18</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>379</v>
+        <v>329</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C12" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A12,Stations!A:A,1,FALSE)=A12,"taken"),"free")</f>
-        <v>free</v>
+        <v>taken</v>
       </c>
       <c r="D12">
         <f>_xlfn.IFNA(VLOOKUP(B12,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.58E+18</v>
+        <v>1.56E+18</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>380</v>
+        <v>330</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C13" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A13,Stations!A:A,1,FALSE)=A13,"taken"),"free")</f>
-        <v>free</v>
+        <v>taken</v>
       </c>
       <c r="D13">
         <f>_xlfn.IFNA(VLOOKUP(B13,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.58E+18</v>
+        <v>1.56E+18</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>387</v>
+        <v>331</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C14" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A14,Stations!A:A,1,FALSE)=A14,"taken"),"free")</f>
-        <v>free</v>
+        <v>taken</v>
       </c>
       <c r="D14">
         <f>_xlfn.IFNA(VLOOKUP(B14,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.58E+18</v>
+        <v>1.56E+18</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>389</v>
+        <v>332</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C15" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A15,Stations!A:A,1,FALSE)=A15,"taken"),"free")</f>
-        <v>free</v>
+        <v>taken</v>
       </c>
       <c r="D15">
         <f>_xlfn.IFNA(VLOOKUP(B15,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.58E+18</v>
+        <v>1.56E+18</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>397</v>
+        <v>334</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C16" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A16,Stations!A:A,1,FALSE)=A16,"taken"),"free")</f>
-        <v>free</v>
+        <v>taken</v>
       </c>
       <c r="D16">
         <f>_xlfn.IFNA(VLOOKUP(B16,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.57E+18</v>
-      </c>
-      <c r="G16" t="s">
-        <v>2579</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.56E+18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>397</v>
+        <v>335</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="C17" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A17,Stations!A:A,1,FALSE)=A17,"taken"),"free")</f>
-        <v>free</v>
-      </c>
-      <c r="D17" t="str">
+        <v>taken</v>
+      </c>
+      <c r="D17">
         <f>_xlfn.IFNA(VLOOKUP(B17,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>not found</v>
-      </c>
-      <c r="E17" t="s">
-        <v>2581</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.56E+18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>404</v>
+        <v>364</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C18" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A18,Stations!A:A,1,FALSE)=A18,"taken"),"free")</f>
-        <v>free</v>
+        <v>taken</v>
       </c>
       <c r="D18">
         <f>_xlfn.IFNA(VLOOKUP(B18,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.59E+18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.56E+18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>459</v>
+        <v>365</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="C19" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A19,Stations!A:A,1,FALSE)=A19,"taken"),"free")</f>
-        <v>free</v>
+        <v>taken</v>
       </c>
       <c r="D19">
         <f>_xlfn.IFNA(VLOOKUP(B19,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>760</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.56E+18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>473</v>
+        <v>366</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C20" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A20,Stations!A:A,1,FALSE)=A20,"taken"),"free")</f>
-        <v>free</v>
+        <v>taken</v>
       </c>
       <c r="D20">
         <f>_xlfn.IFNA(VLOOKUP(B20,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
         <v>1.56E+18</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>512</v>
+        <v>368</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="C21" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A21,Stations!A:A,1,FALSE)=A21,"taken"),"free")</f>
-        <v>free</v>
-      </c>
-      <c r="D21" t="str">
+        <v>taken</v>
+      </c>
+      <c r="D21">
         <f>_xlfn.IFNA(VLOOKUP(B21,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>not found</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.56E+18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>606</v>
+        <v>397</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="C22" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A22,Stations!A:A,1,FALSE)=A22,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D22" t="str">
+      <c r="D22">
         <f>_xlfn.IFNA(VLOOKUP(B22,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>not found</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.57E+18</v>
+      </c>
+      <c r="G22" t="s">
+        <v>2579</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>607</v>
+        <v>371</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C23" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A23,Stations!A:A,1,FALSE)=A23,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D23" t="str">
+      <c r="D23">
         <f>_xlfn.IFNA(VLOOKUP(B23,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>not found</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.58E+18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>608</v>
+        <v>379</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="C24" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A24,Stations!A:A,1,FALSE)=A24,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D24" t="str">
+      <c r="D24">
         <f>_xlfn.IFNA(VLOOKUP(B24,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>not found</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.58E+18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>609</v>
+        <v>380</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C25" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A25,Stations!A:A,1,FALSE)=A25,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D25" t="str">
+      <c r="D25">
         <f>_xlfn.IFNA(VLOOKUP(B25,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>not found</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.58E+18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>610</v>
+        <v>387</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="C26" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A26,Stations!A:A,1,FALSE)=A26,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D26" t="str">
+      <c r="D26">
         <f>_xlfn.IFNA(VLOOKUP(B26,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>not found</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.58E+18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>611</v>
+        <v>389</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="C27" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A27,Stations!A:A,1,FALSE)=A27,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D27" t="str">
+      <c r="D27">
         <f>_xlfn.IFNA(VLOOKUP(B27,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>not found</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.58E+18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>612</v>
+        <v>404</v>
       </c>
       <c r="B28" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C28" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A28,Stations!A:A,1,FALSE)=A28,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D28" t="str">
+      <c r="D28">
         <f>_xlfn.IFNA(VLOOKUP(B28,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>not found</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1.59E+18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>613</v>
+        <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C29" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A29,Stations!A:A,1,FALSE)=A29,"taken"),"free")</f>
@@ -9313,12 +9304,12 @@
         <v>not found</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>613</v>
+        <v>372</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C30" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A30,Stations!A:A,1,FALSE)=A30,"taken"),"free")</f>
@@ -9329,15 +9320,18 @@
         <v>not found</v>
       </c>
       <c r="E30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1195</v>
+      </c>
+      <c r="F30">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>614</v>
+        <v>372</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C31" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A31,Stations!A:A,1,FALSE)=A31,"taken"),"free")</f>
@@ -9348,12 +9342,12 @@
         <v>not found</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>615</v>
+        <v>397</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C32" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A32,Stations!A:A,1,FALSE)=A32,"taken"),"free")</f>
@@ -9363,13 +9357,16 @@
         <f>_xlfn.IFNA(VLOOKUP(B32,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
         <v>not found</v>
       </c>
+      <c r="E32" t="s">
+        <v>2581</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>616</v>
+        <v>512</v>
       </c>
       <c r="B33" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C33" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A33,Stations!A:A,1,FALSE)=A33,"taken"),"free")</f>
@@ -9382,10 +9379,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>617</v>
+        <v>606</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C34" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A34,Stations!A:A,1,FALSE)=A34,"taken"),"free")</f>
@@ -9398,10 +9395,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C35" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A35,Stations!A:A,1,FALSE)=A35,"taken"),"free")</f>
@@ -9414,26 +9411,26 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>651</v>
+        <v>608</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C36" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A36,Stations!A:A,1,FALSE)=A36,"taken"),"free")</f>
         <v>free</v>
       </c>
-      <c r="D36">
+      <c r="D36" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B36,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>674</v>
+        <v>not found</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>669</v>
+        <v>609</v>
       </c>
       <c r="B37" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C37" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A37,Stations!A:A,1,FALSE)=A37,"taken"),"free")</f>
@@ -9446,10 +9443,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>670</v>
+        <v>610</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="C38" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A38,Stations!A:A,1,FALSE)=A38,"taken"),"free")</f>
@@ -9462,10 +9459,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>671</v>
+        <v>611</v>
       </c>
       <c r="B39" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C39" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A39,Stations!A:A,1,FALSE)=A39,"taken"),"free")</f>
@@ -9475,16 +9472,13 @@
         <f>_xlfn.IFNA(VLOOKUP(B39,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
         <v>not found</v>
       </c>
-      <c r="E39" t="s">
-        <v>2580</v>
-      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>675</v>
+        <v>612</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="C40" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A40,Stations!A:A,1,FALSE)=A40,"taken"),"free")</f>
@@ -9497,10 +9491,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>676</v>
+        <v>613</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="C41" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A41,Stations!A:A,1,FALSE)=A41,"taken"),"free")</f>
@@ -9512,8 +9506,11 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>613</v>
+      </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C42" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A42,Stations!A:A,1,FALSE)=A42,"taken"),"free")</f>
@@ -9523,10 +9520,16 @@
         <f>_xlfn.IFNA(VLOOKUP(B42,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
         <v>not found</v>
       </c>
+      <c r="E42" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>614</v>
+      </c>
       <c r="B43" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C43" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A43,Stations!A:A,1,FALSE)=A43,"taken"),"free")</f>
@@ -9538,8 +9541,11 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>615</v>
+      </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C44" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A44,Stations!A:A,1,FALSE)=A44,"taken"),"free")</f>
@@ -9552,181 +9558,175 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>20</v>
+        <v>616</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="C45" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A45,Stations!A:A,1,FALSE)=A45,"taken"),"free")</f>
-        <v>taken</v>
-      </c>
-      <c r="D45">
+        <v>free</v>
+      </c>
+      <c r="D45" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B45,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.52E+18</v>
+        <v>not found</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>329</v>
+        <v>617</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C46" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A46,Stations!A:A,1,FALSE)=A46,"taken"),"free")</f>
-        <v>taken</v>
-      </c>
-      <c r="D46">
+        <v>free</v>
+      </c>
+      <c r="D46" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B46,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.56E+18</v>
+        <v>not found</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>330</v>
+        <v>618</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C47" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A47,Stations!A:A,1,FALSE)=A47,"taken"),"free")</f>
-        <v>taken</v>
-      </c>
-      <c r="D47">
+        <v>free</v>
+      </c>
+      <c r="D47" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B47,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.56E+18</v>
+        <v>not found</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>331</v>
+        <v>669</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="C48" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A48,Stations!A:A,1,FALSE)=A48,"taken"),"free")</f>
-        <v>taken</v>
-      </c>
-      <c r="D48">
+        <v>free</v>
+      </c>
+      <c r="D48" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B48,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.56E+18</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>not found</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>332</v>
+        <v>670</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C49" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A49,Stations!A:A,1,FALSE)=A49,"taken"),"free")</f>
-        <v>taken</v>
-      </c>
-      <c r="D49">
+        <v>free</v>
+      </c>
+      <c r="D49" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B49,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.56E+18</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>not found</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>334</v>
+        <v>671</v>
       </c>
       <c r="B50" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C50" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A50,Stations!A:A,1,FALSE)=A50,"taken"),"free")</f>
-        <v>taken</v>
-      </c>
-      <c r="D50">
+        <v>free</v>
+      </c>
+      <c r="D50" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B50,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.56E+18</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>not found</v>
+      </c>
+      <c r="E50" t="s">
+        <v>2580</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>335</v>
+        <v>675</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C51" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A51,Stations!A:A,1,FALSE)=A51,"taken"),"free")</f>
-        <v>taken</v>
-      </c>
-      <c r="D51">
+        <v>free</v>
+      </c>
+      <c r="D51" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B51,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.56E+18</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>not found</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>364</v>
+        <v>676</v>
       </c>
       <c r="B52" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C52" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A52,Stations!A:A,1,FALSE)=A52,"taken"),"free")</f>
-        <v>taken</v>
-      </c>
-      <c r="D52">
+        <v>free</v>
+      </c>
+      <c r="D52" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B52,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.56E+18</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>365</v>
-      </c>
+        <v>not found</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="C53" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A53,Stations!A:A,1,FALSE)=A53,"taken"),"free")</f>
-        <v>taken</v>
-      </c>
-      <c r="D53">
+        <v>free</v>
+      </c>
+      <c r="D53" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B53,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.56E+18</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>366</v>
-      </c>
+        <v>not found</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="C54" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A54,Stations!A:A,1,FALSE)=A54,"taken"),"free")</f>
-        <v>taken</v>
-      </c>
-      <c r="D54">
+        <v>free</v>
+      </c>
+      <c r="D54" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B54,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.56E+18</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>368</v>
-      </c>
+        <v>not found</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="C55" t="str">
         <f>_xlfn.IFNA(IF(VLOOKUP(A55,Stations!A:A,1,FALSE)=A55,"taken"),"free")</f>
-        <v>taken</v>
-      </c>
-      <c r="D55">
+        <v>free</v>
+      </c>
+      <c r="D55" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B55,Stations!$B$2:$C$1270,2,FALSE),"not found")</f>
-        <v>1.56E+18</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>not found</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>566</v>
       </c>
@@ -9742,7 +9742,7 @@
         <v>not found</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>625</v>
       </c>
@@ -9758,7 +9758,7 @@
         <v>not found</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>704</v>
       </c>
@@ -9775,11 +9775,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G58" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G58">
-      <sortCondition ref="C1:C58"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:G58" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="free">
       <formula>NOT(ISERROR(SEARCH("free",C1)))</formula>

</xml_diff>